<commit_message>
Site updated: 2022-01-19 13:28:54
</commit_message>
<xml_diff>
--- a/2019/08/09/matplotlib绘制势能面剖面图/EnergyProfile.xlsx
+++ b/2019/08/09/matplotlib绘制势能面剖面图/EnergyProfile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D1589-B228-4907-B604-6C9659A43C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C499115-A422-459B-A550-3FDBBD35C1F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2270" yWindow="1800" windowWidth="25670" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,25 +82,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pic_title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Relative Energy Profile along the reaction path</t>
-  </si>
-  <si>
-    <t>Reaction coordinate</t>
-  </si>
-  <si>
-    <t>X_title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y_title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Relative Energy(eV)</t>
+    <t>linestyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -111,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,11 +119,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -158,17 +143,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -463,168 +447,153 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-0.8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
         <v>0.1</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="C7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
         <v>-0.5</v>
       </c>
-      <c r="C8" s="3">
-        <v>-0.8</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C9" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.2</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D10" s="1">
         <v>-0.7</v>
       </c>
-      <c r="D10" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="C11" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3">
-        <v>-1.5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>-0.7</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>